<commit_message>
Stellingen en opdrachten van BvT
</commit_message>
<xml_diff>
--- a/LESWEEK4/opdrachten/Opdrachten_week_4.xlsx
+++ b/LESWEEK4/opdrachten/Opdrachten_week_4.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bartvantrigt/Dropbox/031_GIT/LESWEEK4/opdrachten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bartvantrigt/Dropbox/031_GIT (1)/LESWEEK4/opdrachten/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="week2_1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">week2_1!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">week4_1!$A$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="150000" calcMode="manual" calcCompleted="0" concurrentCalc="0"/>
+  <calcPr calcId="150000" calcMode="manual" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="129">
   <si>
     <t>vraag</t>
   </si>
@@ -363,6 +363,93 @@
   </si>
   <si>
     <t>hallo A= 712884+912831+812873</t>
+  </si>
+  <si>
+    <t>indices</t>
+  </si>
+  <si>
+    <t>Wanneer je een index -1 op vraagt krijg je een foutmelding</t>
+  </si>
+  <si>
+    <t>Wanneer je een index -1 op vraagt krijg je geen foutmelding</t>
+  </si>
+  <si>
+    <t>Wanneer je een index 1.1231 op vraagt krijg je een foutmelding</t>
+  </si>
+  <si>
+    <t>Wanneer je een index 3 op vraagt van de vector v=[1 2 3] krijg je een foutmelding</t>
+  </si>
+  <si>
+    <t>Wanneer je een index 1.1 op vraagt van de vector v=[1.1 1.2 1.3] krijg je een foutmelding</t>
+  </si>
+  <si>
+    <t>indices v2</t>
+  </si>
+  <si>
+    <t>Wanneer je een index (1,3) op vraagt van de vector v=[1.1 1.2 1.3] krijg je een foutmelding</t>
+  </si>
+  <si>
+    <t>Wanneer je een index (3,1) op vraagt van de vector v=[1.1 1.2 1.3] krijg je een foutmelding</t>
+  </si>
+  <si>
+    <t>Wanneer je een index (1,1) op vraagt van de vector v=[1.1 1.2 1.3] krijg je een foutmelding</t>
+  </si>
+  <si>
+    <t>Wanneer je een index (1,4) op vraagt van de vector v=[1.1 1.2 1.3] krijg je een foutmelding</t>
+  </si>
+  <si>
+    <t>Wanneer je een index 1 op vraagt van de vector v=[1 2 3] krijg je een foutmelding</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>Wanneer je wilt controleren of twee variabele aan elkaar gelijk zijn moet je een '=' tekens gebruiken</t>
+  </si>
+  <si>
+    <t>Wanneer je wilt controleren of twee variabele aan elkaar gelijk zijn moet je twee '=' tekens gebruiken</t>
+  </si>
+  <si>
+    <t>hallo if n&lt;5 x=3 elseif n==5 x=5  else x=10 end</t>
+  </si>
+  <si>
+    <t>hallo if n==1 x=3 elseif n&gt;3 x=4 else x=3 end</t>
+  </si>
+  <si>
+    <t>hallo if n==1 x=3 elseif n&lt;3 x=4 else x=3 end</t>
+  </si>
+  <si>
+    <t>hallo if n==1 x=3 elseif n=3 x=4 else x=3 end</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3 </t>
+  </si>
+  <si>
+    <t>CHECKEN!</t>
+  </si>
+  <si>
+    <t>hallo Matrix=[ 78 127 28; 291 29 12; 92 19 0]; Matrix(3,127)</t>
+  </si>
+  <si>
+    <t>hallo Matrix=[ 78 127 28; 291 29 12; 92 19 0]; Matrix(1,3) = 32</t>
+  </si>
+  <si>
+    <t>hallo Matrix=[ 78 127 28; 291 29 12; 92 19 0]; Matrix(1,3) = [32 21 32]</t>
+  </si>
+  <si>
+    <t>hallo Matrix=[ 78 127 28; 291 29 12; 92 19 0]; Matrix(1,1:3) = [32 21 32]</t>
+  </si>
+  <si>
+    <t>hallo Matrix=[ 78 127 28; 291 29 12; 92 19 0]; Matrix(1:3,1) = [32 21 32]</t>
+  </si>
+  <si>
+    <t>3.6</t>
   </si>
 </sst>
 </file>
@@ -415,12 +502,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -432,7 +525,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -472,8 +565,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -491,8 +608,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -512,6 +641,18 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -531,6 +672,18 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1549,11 +1702,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F96"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1601,6 +1754,9 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>80</v>
       </c>
@@ -1701,22 +1857,10 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="2" t="b">
-        <v>1</v>
-      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="2" t="b">
-        <v>0</v>
-      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
@@ -1740,293 +1884,372 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" s="2" t="b">
-        <v>1</v>
-      </c>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C19" s="2" t="b">
-        <v>0</v>
-      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="2" t="b">
-        <v>1</v>
-      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="2" t="b">
-        <v>0</v>
-      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="2" t="b">
+      <c r="C22" s="7" t="b">
         <v>1</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C23" s="2" t="b">
+      <c r="C23" s="7" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="2"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="2"/>
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="C26" s="2"/>
+      <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="C27" s="2"/>
+    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="2"/>
+        <v>106</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="2"/>
+        <v>106</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="2"/>
+        <v>106</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="2"/>
+        <v>106</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
-      <c r="C34" s="2"/>
+    <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>52</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="4"/>
-      <c r="C36" s="2"/>
+    <row r="36" spans="1:5" ht="11" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
-      <c r="C38" s="2"/>
+      <c r="B38" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="2"/>
+      <c r="B39" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>8</v>
-      </c>
-      <c r="C40" s="2"/>
+      <c r="B40" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
-      <c r="C41" s="2"/>
+      <c r="B41" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
-      <c r="C42" s="2"/>
+      <c r="B42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="1"/>
-      <c r="C43" s="2"/>
+    <row r="43" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" s="2"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="C45" s="2"/>
+      <c r="B45" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="B46" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>25</v>
-      </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="2"/>
+      <c r="B47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>31</v>
-      </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="2"/>
+      <c r="B48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>33</v>
-      </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="2"/>
+    <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C49" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B50" s="1"/>
-      <c r="C50" s="2"/>
+    <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>37</v>
-      </c>
-      <c r="B51" s="1"/>
-      <c r="C51" s="2"/>
+    <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="2"/>
@@ -2034,212 +2257,481 @@
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>41</v>
-      </c>
       <c r="B53" s="1"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>68</v>
-      </c>
       <c r="B54" s="1"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>52</v>
-      </c>
       <c r="B55" s="1"/>
       <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
       <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>53</v>
-      </c>
       <c r="B56" s="1"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B58" s="1"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="1"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>27</v>
-      </c>
-      <c r="B61" s="1"/>
+      <c r="A61" s="3"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>30</v>
-      </c>
-      <c r="B62" s="1"/>
+      <c r="A62" s="3"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>31</v>
       </c>
       <c r="B63" s="1"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>33</v>
       </c>
       <c r="B64" s="1"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>37</v>
       </c>
       <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>38</v>
       </c>
       <c r="B66" s="1"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>41</v>
       </c>
       <c r="B67" s="1"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B69" s="1"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B71" s="4"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B73" s="1"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>69</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>8</v>
+      </c>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B76" s="1"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B77" s="1"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B78" s="1"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B79" t="s">
+        <v>72</v>
+      </c>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="3"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>25</v>
+      </c>
+      <c r="B82" s="1"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>31</v>
+      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>33</v>
+      </c>
+      <c r="B84" s="1"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B85" s="1"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B86" s="1"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87" s="1"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>41</v>
+      </c>
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>68</v>
+      </c>
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>52</v>
+      </c>
+      <c r="B90" s="1"/>
+      <c r="C90" s="2"/>
+      <c r="E90" s="2"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>53</v>
+      </c>
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>25</v>
+      </c>
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>27</v>
+      </c>
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>30</v>
+      </c>
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>31</v>
+      </c>
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>33</v>
+      </c>
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>37</v>
+      </c>
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>38</v>
+      </c>
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>41</v>
+      </c>
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>44</v>
       </c>
-      <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="B103" s="1"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>47</v>
       </c>
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="B104" s="1"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>49</v>
       </c>
-      <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="B105" s="1"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>52</v>
       </c>
-      <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="B106" s="1"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>53</v>
       </c>
-      <c r="B72" s="1"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="B107" s="1"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>56</v>
       </c>
-      <c r="B73" s="1"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="B108" s="1"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>51</v>
       </c>
-      <c r="B74" s="1"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="B109" s="1"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>63</v>
       </c>
-      <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="B110" s="1"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>64</v>
       </c>
-      <c r="B76" s="1"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="B111" s="1"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>66</v>
       </c>
-      <c r="B77" s="1"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B83" s="1"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B84" s="1"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B85" s="1"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B86" s="1"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B87" s="1"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B90" s="1"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B91" s="1"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="5" t="s">
+      <c r="B112" s="1"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B123" s="1"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B124" s="1"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B125" s="1"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B126" s="1"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B127" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B93" s="1" t="s">
+    <row r="128" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B128" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B94" s="1" t="s">
+      <c r="E128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="B129" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F129" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B95" s="1"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B96" s="1"/>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B130" s="1"/>
+    </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B131" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1"/>

</xml_diff>